<commit_message>
CIERRE 12 ENE 24
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL#16   ARCHIVO   2 0 2 3/I R A N A   2023.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL#16   ARCHIVO   2 0 2 3/I R A N A   2023.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="12">
   <si>
     <t xml:space="preserve">GASTOS DE  AGUA   SENDEROS        I R A N A </t>
   </si>
@@ -600,7 +600,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
+      <selection pane="bottomLeft" activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1724,12 +1724,18 @@
       </c>
     </row>
     <row r="79" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B79" s="2"/>
-      <c r="C79" s="19"/>
-      <c r="D79" s="6"/>
+      <c r="B79" s="2">
+        <v>45300</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" s="6">
+        <v>-212</v>
+      </c>
       <c r="E79" s="6">
         <f t="shared" si="1"/>
-        <v>398</v>
+        <v>186</v>
       </c>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.3">
@@ -1738,7 +1744,7 @@
       <c r="D80" s="6"/>
       <c r="E80" s="6">
         <f t="shared" si="1"/>
-        <v>398</v>
+        <v>186</v>
       </c>
     </row>
     <row r="81" spans="2:5" x14ac:dyDescent="0.3">
@@ -1747,7 +1753,7 @@
       <c r="D81" s="6"/>
       <c r="E81" s="6">
         <f t="shared" si="1"/>
-        <v>398</v>
+        <v>186</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.3">
@@ -1756,7 +1762,7 @@
       <c r="D82" s="6"/>
       <c r="E82" s="6">
         <f t="shared" si="1"/>
-        <v>398</v>
+        <v>186</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.3">

</xml_diff>